<commit_message>
feat：change environment color set
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/SceneEnvironment_场景环境表.xlsx
+++ b/dragon-verse/Excels/SceneEnvironment_场景环境表.xlsx
@@ -111,21 +111,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="175">
   <si>
     <t xml:space="preserve">int</t>
   </si>
   <si>
-    <t xml:space="preserve">vector4</t>
+    <t xml:space="preserve">string</t>
   </si>
   <si>
     <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vector4</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -517,121 +511,133 @@
     <t xml:space="preserve">天光颜色</t>
   </si>
   <si>
-    <t xml:space="preserve">1.000000|1.000000|1.000000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.052106|0.242233|0.944853|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.066626|0.152926|0.921582|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.018860|0.050527|0.305147|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.686685|0.304987|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.063010|0.246201|0.434154|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000000|0.000000|0.000000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|1.000000|1.000000|0.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.917647|0.917647|1.000000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.729412|0.815686|0.952941|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.737255|0.737255|0.737255|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.427451|0.635294|0.882353|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.231373|0.458824|0.776471|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.886275|0.713725|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.784314|0.894118|0.980392|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.768627|0.584314|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.800000|0.596078|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.882353|0.721569|0.764706|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.392157|0.411765|0.776471|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.890196|0.611765|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.933333|0.858824|0.858824|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.721569|0.776471|1.000000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.631373|0.717647|0.952941|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.403922|0.611765|0.964706|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.137255|0.352941|0.905882|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|1.000000|1.000000|0.950000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.882353|0.800000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.921569|0.843137|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.980392|0.972549|0.949020|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.894118|0.917647|1.000000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.737255|0.737255|0.737255|0.737255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.603922|0.698039|0.952941|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.192157|0.317647|0.733333|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.811765|0.847059|1.000000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.752941|0.376471|0.552941|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000000|0.811765|1.000000|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.388235|0.329412|0.403922|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.529412|0.635294|0.780392|1.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.988235|0.737255|0.996078|0.000000</t>
+    <t xml:space="preserve">255|255|255|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13|62|241|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17|39|235|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5|13|78|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|175|78|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16|63|111|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|0|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|255|255|0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">235|235|255|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">186|208|243|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">188|188|188|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109|162|225|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59|117|198|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|226|182|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200|228|250|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|197|150|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|204|152|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">225|184|195|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100|105|198|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|227|156|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">238|219|219|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">185|199|255|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">161|183|243|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103|156|246|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35|90|231|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|255|255|242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|226|204|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|235|215|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250|248|242|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">228|235|255|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">188|188|188|188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">154|178|243|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49|81|187|255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">207|216|255|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">192|96|141|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|207|255|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">99|84|103|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|0|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|226|182|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16|63|111|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">135|162|199|255 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">252|188|254|0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255|255|255|0 </t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -746,15 +752,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -782,7 +784,7 @@
   <dimension ref="A1:BO46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -791,24 +793,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="16.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="45.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="34.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="24.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="50.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="36.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="50.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="51.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="37.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="16.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="41.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="41.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="44.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="37.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="33.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="36.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="50.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="51.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="37.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="41.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="41.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="1" width="44.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="37.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="33.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="10.94"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,7 +833,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
@@ -846,7 +848,7 @@
         <v>2</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
@@ -873,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>1</v>
@@ -885,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>0</v>
@@ -900,7 +902,7 @@
         <v>2</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE1" s="3" t="s">
         <v>0</v>
@@ -951,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="AU1" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>2</v>
@@ -1010,393 +1012,393 @@
     </row>
     <row r="2" s="3" customFormat="true" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BE2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BF2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BG2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BH2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BI2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BK2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="BJ2" s="3" t="s">
+      <c r="BL2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="BK2" s="3" t="s">
+      <c r="BM2" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="BM2" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="true" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AM3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AN3" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AO3" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AN3" s="3" t="s">
+      <c r="AP3" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AP3" s="3" t="s">
+      <c r="AR3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="AQ3" s="3" t="s">
+      <c r="AS3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="AR3" s="3" t="s">
+      <c r="AT3" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AU3" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="AT3" s="3" t="s">
+      <c r="AV3" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="AU3" s="3" t="s">
+      <c r="AW3" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="AV3" s="3" t="s">
+      <c r="AX3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="AW3" s="3" t="s">
+      <c r="AY3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="AX3" s="3" t="s">
+      <c r="AZ3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="AY3" s="3" t="s">
+      <c r="BA3" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="BB3" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="BA3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BD3" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="BC3" s="3" t="s">
+      <c r="BE3" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="BD3" s="3" t="s">
+      <c r="BF3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="BE3" s="3" t="s">
+      <c r="BG3" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="BF3" s="3" t="s">
+      <c r="BH3" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="BG3" s="3" t="s">
+      <c r="BI3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="BH3" s="3" t="s">
+      <c r="BJ3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="BI3" s="3" t="s">
+      <c r="BK3" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="BJ3" s="3" t="s">
+      <c r="BL3" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="BK3" s="3" t="s">
+      <c r="BM3" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="BL3" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="BM3" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="4" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1408,192 +1410,192 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>178196</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="8" t="n">
+        <v>5.23</v>
+      </c>
+      <c r="S5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <v>178196</v>
-      </c>
-      <c r="H5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="7" t="n">
+      <c r="U5" s="8" t="n">
+        <v>209510</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="7" t="n">
-        <v>5.23</v>
-      </c>
-      <c r="S5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="7" t="s">
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="U5" s="7" t="n">
-        <v>209510</v>
-      </c>
-      <c r="V5" s="7" t="s">
+      <c r="AB5" s="8" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC5" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD5" s="8" t="n">
+        <v>14309</v>
+      </c>
+      <c r="AE5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="8" t="n">
+        <v>137.93</v>
+      </c>
+      <c r="AG5" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH5" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI5" s="8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AJ5" s="8" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AK5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="8" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AS5" s="8" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="AT5" s="8" t="n">
+        <v>-361.83</v>
+      </c>
+      <c r="AU5" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="W5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="X5" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="7" t="s">
+      <c r="AV5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="8" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AX5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AB5" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC5" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD5" s="7" t="n">
-        <v>14309</v>
-      </c>
-      <c r="AE5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="7" t="n">
-        <v>137.93</v>
-      </c>
-      <c r="AG5" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AH5" s="7" t="n">
+      <c r="BA5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="8" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="BC5" s="8" t="n">
+        <v>-27.81</v>
+      </c>
+      <c r="BD5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="BE5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG5" s="8" t="n">
+        <v>7500</v>
+      </c>
+      <c r="BH5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI5" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="BJ5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="AI5" s="7" t="n">
+      <c r="BK5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="BL5" s="8" t="n">
         <v>1.5</v>
       </c>
-      <c r="AJ5" s="7" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="AK5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AP5" s="7"/>
-      <c r="AQ5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR5" s="7" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="AS5" s="7" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="AT5" s="7" t="n">
-        <v>-361.83</v>
-      </c>
-      <c r="AU5" s="7" t="s">
+      <c r="BM5" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AV5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="7" t="n">
-        <v>4000</v>
-      </c>
-      <c r="AX5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="BA5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB5" s="7" t="n">
-        <v>5.02</v>
-      </c>
-      <c r="BC5" s="7" t="n">
-        <v>-27.81</v>
-      </c>
-      <c r="BD5" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="BE5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="BG5" s="7" t="n">
-        <v>7500</v>
-      </c>
-      <c r="BH5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="BI5" s="7" t="n">
-        <v>6000</v>
-      </c>
-      <c r="BJ5" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="BK5" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="BL5" s="7" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="BM5" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="BN5" s="0"/>
-      <c r="BO5" s="0"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>142</v>
+      <c r="A6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>1</v>
@@ -1611,7 +1613,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J6" s="4" t="n">
         <v>5</v>
@@ -1628,11 +1630,11 @@
       <c r="N6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="4" t="s">
-        <v>143</v>
+      <c r="O6" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q6" s="4" t="n">
         <v>1</v>
@@ -1643,14 +1645,14 @@
       <c r="S6" s="4" t="n">
         <v>1.17</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>145</v>
+      <c r="T6" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="U6" s="4" t="n">
         <v>195714</v>
       </c>
-      <c r="V6" s="4" t="s">
-        <v>146</v>
+      <c r="V6" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="W6" s="4" t="n">
         <v>0.68</v>
@@ -1661,8 +1663,8 @@
       <c r="Z6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AA6" s="4" t="s">
-        <v>147</v>
+      <c r="AA6" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="AB6" s="4" t="n">
         <v>40</v>
@@ -1709,8 +1711,8 @@
       <c r="AT6" s="4" t="n">
         <v>-361.83</v>
       </c>
-      <c r="AU6" s="4" t="s">
-        <v>139</v>
+      <c r="AU6" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="AV6" s="4" t="n">
         <v>1</v>
@@ -1724,8 +1726,8 @@
       <c r="AY6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AZ6" s="4" t="s">
-        <v>140</v>
+      <c r="AZ6" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="BA6" s="4" t="n">
         <v>0</v>
@@ -1736,8 +1738,8 @@
       <c r="BC6" s="4" t="n">
         <v>32.74</v>
       </c>
-      <c r="BD6" s="4" t="s">
-        <v>148</v>
+      <c r="BD6" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="BE6" s="4" t="n">
         <v>-1.36</v>
@@ -1757,14 +1759,14 @@
       <c r="BJ6" s="4" t="n">
         <v>44.96</v>
       </c>
-      <c r="BK6" s="4" t="s">
-        <v>141</v>
+      <c r="BK6" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="BL6" s="4" t="n">
         <v>1.62</v>
       </c>
       <c r="BM6" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,8 +1776,8 @@
       <c r="B7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>149</v>
+      <c r="C7" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>1</v>
@@ -1793,7 +1795,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J7" s="4" t="n">
         <v>1</v>
@@ -1810,11 +1812,11 @@
       <c r="N7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>134</v>
+      <c r="O7" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="Q7" s="4" t="n">
         <v>1</v>
@@ -1825,14 +1827,14 @@
       <c r="S7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T7" s="4" t="s">
-        <v>151</v>
+      <c r="T7" s="7" t="s">
+        <v>149</v>
       </c>
       <c r="U7" s="4" t="n">
         <v>108338</v>
       </c>
-      <c r="V7" s="4" t="s">
-        <v>152</v>
+      <c r="V7" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="W7" s="4" t="n">
         <v>1</v>
@@ -1846,8 +1848,8 @@
       <c r="Z7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AA7" s="4" t="s">
-        <v>153</v>
+      <c r="AA7" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="AB7" s="4" t="n">
         <v>20</v>
@@ -1894,8 +1896,8 @@
       <c r="AT7" s="4" t="n">
         <v>-361.83</v>
       </c>
-      <c r="AU7" s="4" t="s">
-        <v>139</v>
+      <c r="AU7" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="AV7" s="4" t="n">
         <v>1</v>
@@ -1909,8 +1911,8 @@
       <c r="AY7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AZ7" s="4" t="s">
-        <v>140</v>
+      <c r="AZ7" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="BA7" s="4" t="n">
         <v>0</v>
@@ -1921,8 +1923,8 @@
       <c r="BC7" s="4" t="n">
         <v>-20</v>
       </c>
-      <c r="BD7" s="4" t="s">
-        <v>154</v>
+      <c r="BD7" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="BE7" s="4" t="n">
         <v>0</v>
@@ -1942,25 +1944,25 @@
       <c r="BJ7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="BK7" s="4" t="s">
-        <v>141</v>
+      <c r="BK7" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="BL7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="BM7" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
+      <c r="A8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>155</v>
+      <c r="C8" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>1</v>
@@ -1978,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J8" s="4" t="n">
         <v>5</v>
@@ -1995,11 +1997,11 @@
       <c r="N8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>134</v>
+      <c r="O8" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="Q8" s="4" t="n">
         <v>1</v>
@@ -2010,14 +2012,14 @@
       <c r="S8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T8" s="4" t="s">
-        <v>157</v>
+      <c r="T8" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="U8" s="4" t="n">
         <v>108338</v>
       </c>
-      <c r="V8" s="4" t="s">
-        <v>158</v>
+      <c r="V8" s="7" t="s">
+        <v>156</v>
       </c>
       <c r="W8" s="4" t="n">
         <v>1</v>
@@ -2028,8 +2030,8 @@
       <c r="Z8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" s="4" t="s">
-        <v>147</v>
+      <c r="AA8" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="AB8" s="4" t="n">
         <v>1</v>
@@ -2076,8 +2078,8 @@
       <c r="AT8" s="4" t="n">
         <v>-361.83</v>
       </c>
-      <c r="AU8" s="4" t="s">
-        <v>139</v>
+      <c r="AU8" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="AV8" s="4" t="n">
         <v>1</v>
@@ -2091,8 +2093,8 @@
       <c r="AY8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AZ8" s="4" t="s">
-        <v>140</v>
+      <c r="AZ8" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="BA8" s="4" t="n">
         <v>0</v>
@@ -2103,8 +2105,8 @@
       <c r="BC8" s="4" t="n">
         <v>-50</v>
       </c>
-      <c r="BD8" s="4" t="s">
-        <v>159</v>
+      <c r="BD8" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="BE8" s="4" t="n">
         <v>0</v>
@@ -2124,14 +2126,14 @@
       <c r="BJ8" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="BK8" s="4" t="s">
-        <v>141</v>
+      <c r="BK8" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="BL8" s="4" t="n">
         <v>1</v>
       </c>
       <c r="BM8" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,8 +2143,8 @@
       <c r="B9" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>160</v>
+      <c r="C9" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>1</v>
@@ -2160,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J9" s="4" t="n">
         <v>5</v>
@@ -2177,11 +2179,11 @@
       <c r="N9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>144</v>
+      <c r="O9" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="Q9" s="4" t="n">
         <v>1</v>
@@ -2192,14 +2194,14 @@
       <c r="S9" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T9" s="4" t="s">
-        <v>151</v>
+      <c r="T9" s="7" t="s">
+        <v>149</v>
       </c>
       <c r="U9" s="4" t="n">
         <v>59838</v>
       </c>
-      <c r="V9" s="4" t="s">
-        <v>146</v>
+      <c r="V9" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="W9" s="4" t="n">
         <v>1</v>
@@ -2210,8 +2212,8 @@
       <c r="Z9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AA9" s="4" t="s">
-        <v>153</v>
+      <c r="AA9" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="AB9" s="4" t="n">
         <v>20</v>
@@ -2258,8 +2260,8 @@
       <c r="AT9" s="4" t="n">
         <v>-361.83</v>
       </c>
-      <c r="AU9" s="4" t="s">
-        <v>139</v>
+      <c r="AU9" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="AV9" s="4" t="n">
         <v>1</v>
@@ -2273,8 +2275,8 @@
       <c r="AY9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AZ9" s="4" t="s">
-        <v>140</v>
+      <c r="AZ9" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="BA9" s="4" t="n">
         <v>0</v>
@@ -2285,8 +2287,8 @@
       <c r="BC9" s="4" t="n">
         <v>-75.54</v>
       </c>
-      <c r="BD9" s="4" t="s">
-        <v>162</v>
+      <c r="BD9" s="7" t="s">
+        <v>160</v>
       </c>
       <c r="BE9" s="4" t="n">
         <v>-1.24</v>
@@ -2306,25 +2308,25 @@
       <c r="BJ9" s="4" t="n">
         <v>1.17</v>
       </c>
-      <c r="BK9" s="4" t="s">
-        <v>141</v>
+      <c r="BK9" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="BL9" s="4" t="n">
         <v>1.4</v>
       </c>
       <c r="BM9" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="n">
+      <c r="A10" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>163</v>
+      <c r="C10" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>1</v>
@@ -2342,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J10" s="4" t="n">
         <v>5</v>
@@ -2359,11 +2361,11 @@
       <c r="N10" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>164</v>
+      <c r="O10" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="Q10" s="4" t="n">
         <v>1</v>
@@ -2374,14 +2376,14 @@
       <c r="S10" s="4" t="n">
         <v>1.17</v>
       </c>
-      <c r="T10" s="4" t="s">
-        <v>165</v>
+      <c r="T10" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="U10" s="4" t="n">
         <v>195714</v>
       </c>
-      <c r="V10" s="4" t="s">
-        <v>166</v>
+      <c r="V10" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="W10" s="4" t="n">
         <v>1</v>
@@ -2392,8 +2394,8 @@
       <c r="Z10" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AA10" s="4" t="s">
-        <v>147</v>
+      <c r="AA10" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="AB10" s="4" t="n">
         <v>40</v>
@@ -2413,10 +2415,10 @@
       <c r="AG10" s="4" t="n">
         <v>-1</v>
       </c>
-      <c r="AH10" s="10" t="n">
+      <c r="AH10" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="AI10" s="10" t="n">
+      <c r="AI10" s="9" t="n">
         <v>1.2</v>
       </c>
       <c r="AJ10" s="4" t="n">
@@ -2440,8 +2442,8 @@
       <c r="AT10" s="4" t="n">
         <v>-361.83</v>
       </c>
-      <c r="AU10" s="4" t="s">
-        <v>139</v>
+      <c r="AU10" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="AV10" s="4" t="n">
         <v>1</v>
@@ -2455,8 +2457,8 @@
       <c r="AY10" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AZ10" s="4" t="s">
-        <v>140</v>
+      <c r="AZ10" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="BA10" s="4" t="n">
         <v>0</v>
@@ -2467,8 +2469,8 @@
       <c r="BC10" s="4" t="n">
         <v>-50</v>
       </c>
-      <c r="BD10" s="4" t="s">
-        <v>134</v>
+      <c r="BD10" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="BE10" s="4" t="n">
         <v>0</v>
@@ -2488,14 +2490,14 @@
       <c r="BJ10" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="BK10" s="4" t="s">
-        <v>141</v>
+      <c r="BK10" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="BL10" s="4" t="n">
         <v>1</v>
       </c>
       <c r="BM10" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,8 +2507,8 @@
       <c r="B11" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>167</v>
+      <c r="C11" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="D11" s="4" t="n">
         <v>1</v>
@@ -2523,8 +2525,8 @@
       <c r="H11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>168</v>
+      <c r="I11" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="J11" s="4" t="n">
         <v>2</v>
@@ -2541,11 +2543,11 @@
       <c r="N11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O11" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>169</v>
+      <c r="O11" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="Q11" s="4" t="n">
         <v>1</v>
@@ -2556,14 +2558,14 @@
       <c r="S11" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="T11" s="4" t="s">
-        <v>170</v>
+      <c r="T11" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="U11" s="4" t="n">
         <v>59821</v>
       </c>
-      <c r="V11" s="4" t="s">
-        <v>140</v>
+      <c r="V11" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="W11" s="4" t="n">
         <v>0.72</v>
@@ -2577,8 +2579,8 @@
       <c r="Z11" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AA11" s="4" t="s">
-        <v>147</v>
+      <c r="AA11" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="AB11" s="4" t="n">
         <v>40</v>
@@ -2625,8 +2627,8 @@
       <c r="AT11" s="4" t="n">
         <v>-361.83</v>
       </c>
-      <c r="AU11" s="4" t="s">
-        <v>139</v>
+      <c r="AU11" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="AV11" s="4" t="n">
         <v>1</v>
@@ -2640,8 +2642,8 @@
       <c r="AY11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="AZ11" s="4" t="s">
-        <v>140</v>
+      <c r="AZ11" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="BA11" s="4" t="n">
         <v>0</v>
@@ -2652,8 +2654,8 @@
       <c r="BC11" s="4" t="n">
         <v>-1.73</v>
       </c>
-      <c r="BD11" s="4" t="s">
-        <v>171</v>
+      <c r="BD11" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="BE11" s="4" t="n">
         <v>-0.65</v>
@@ -2673,73 +2675,73 @@
       <c r="BJ11" s="4" t="n">
         <v>44.96</v>
       </c>
-      <c r="BK11" s="4" t="s">
-        <v>172</v>
+      <c r="BK11" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="BL11" s="4" t="n">
         <v>1</v>
       </c>
       <c r="BM11" s="7" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
feat:update environment change and UI
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/SceneEnvironment_场景环境表.xlsx
+++ b/dragon-verse/Excels/SceneEnvironment_场景环境表.xlsx
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="182">
   <si>
     <t>int</t>
   </si>
@@ -530,40 +530,49 @@
     <t>255|175|78|255</t>
   </si>
   <si>
+    <t>(R=0.062526,G=0.247767,B=0.433824,A=1.000000)</t>
+  </si>
+  <si>
+    <t>(R=0.000000,G=0.000000,B=0.000000,A=1.000000)</t>
+  </si>
+  <si>
+    <t>(R=1.000000,G=1.000000,B=1.000000,A=1.000000)</t>
+  </si>
+  <si>
+    <t>255|255|255|0</t>
+  </si>
+  <si>
+    <t>235|235|255|255</t>
+  </si>
+  <si>
+    <t>186|208|243|255</t>
+  </si>
+  <si>
+    <t>188|188|188|255</t>
+  </si>
+  <si>
+    <t>109|162|225|255</t>
+  </si>
+  <si>
+    <t>59|117|198|255</t>
+  </si>
+  <si>
+    <t>255|226|182|255</t>
+  </si>
+  <si>
     <t>16|63|111|255</t>
   </si>
   <si>
     <t>0|0|0|255</t>
   </si>
   <si>
-    <t>255|255|255|0</t>
-  </si>
-  <si>
-    <t>235|235|255|255</t>
-  </si>
-  <si>
-    <t>186|208|243|255</t>
-  </si>
-  <si>
-    <t>188|188|188|255</t>
-  </si>
-  <si>
-    <t>109|162|225|255</t>
-  </si>
-  <si>
-    <t>59|117|198|255</t>
-  </si>
-  <si>
-    <t>255|226|182|255</t>
-  </si>
-  <si>
     <t>200|228|250|255</t>
   </si>
   <si>
     <t>255|197|150|255</t>
   </si>
   <si>
-    <t>255|204|152|255</t>
+    <t>255|204|155|255</t>
   </si>
   <si>
     <t>225|184|195|255</t>
@@ -596,7 +605,16 @@
     <t>255|226|204|255</t>
   </si>
   <si>
-    <t>255|235|215|255</t>
+    <t>(R=1.000000,G=0.830770,B=0.679543,A=1.000000)</t>
+  </si>
+  <si>
+    <t>(R=0.500000,G=0.500000,B=0.500000,A=1.000000)</t>
+  </si>
+  <si>
+    <t>(R=0.752942,G=0.479320,B=0.545725,A=1.000000)</t>
+  </si>
+  <si>
+    <t>(R=0.127438,G=0.141263,B=0.564712,A=1.000000)</t>
   </si>
   <si>
     <t>250|248|242|255</t>
@@ -627,9 +645,6 @@
   </si>
   <si>
     <t>(R=0.124772,G=0.088656,B=0.135633,A=1.000000)</t>
-  </si>
-  <si>
-    <t>(R=0.000000,G=0.000000,B=0.000000,A=1.000000)</t>
   </si>
   <si>
     <t xml:space="preserve">255|226|182|255 </t>
@@ -1830,8 +1845,8 @@
   <sheetPr/>
   <dimension ref="A1:BO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16.5"/>
@@ -2487,7 +2502,9 @@
       <c r="M5" s="8">
         <v>0</v>
       </c>
-      <c r="N5" s="8"/>
+      <c r="N5" s="8">
+        <v>0</v>
+      </c>
       <c r="O5" s="7" t="s">
         <v>133</v>
       </c>
@@ -2602,7 +2619,7 @@
         <v>-27.81</v>
       </c>
       <c r="BD5" s="7" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="BE5" s="8">
         <v>0</v>
@@ -2623,13 +2640,13 @@
         <v>4</v>
       </c>
       <c r="BK5" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL5" s="8">
         <v>1.5</v>
       </c>
       <c r="BM5" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BN5" s="3"/>
       <c r="BO5" s="3"/>
@@ -2642,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -2678,10 +2695,10 @@
         <v>0</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q6" s="2">
         <v>1</v>
@@ -2693,13 +2710,13 @@
         <v>1.17</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U6" s="2">
         <v>195714</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="W6" s="2">
         <v>0.68</v>
@@ -2711,7 +2728,7 @@
         <v>0</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AB6" s="2">
         <v>40</v>
@@ -2759,7 +2776,7 @@
         <v>-361.83</v>
       </c>
       <c r="AU6" s="7" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="AV6" s="2">
         <v>1</v>
@@ -2774,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="AZ6" s="7" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="BA6" s="2">
         <v>0</v>
@@ -2786,7 +2803,7 @@
         <v>32.74</v>
       </c>
       <c r="BD6" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="BE6" s="2">
         <v>-1.36</v>
@@ -2807,13 +2824,13 @@
         <v>44.96</v>
       </c>
       <c r="BK6" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL6" s="2">
         <v>1.62</v>
       </c>
       <c r="BM6" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:65">
@@ -2824,7 +2841,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -2860,7 +2877,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>132</v>
@@ -2875,13 +2892,13 @@
         <v>1</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="U7" s="2">
-        <v>108338</v>
+        <v>14304</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="W7" s="2">
         <v>1</v>
@@ -2896,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="AA7" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AB7" s="2">
         <v>20</v>
@@ -2944,7 +2961,7 @@
         <v>-361.83</v>
       </c>
       <c r="AU7" s="7" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="AV7" s="2">
         <v>1</v>
@@ -2959,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="AZ7" s="7" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="BA7" s="2">
         <v>0</v>
@@ -2971,7 +2988,7 @@
         <v>-20</v>
       </c>
       <c r="BD7" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="BE7" s="2">
         <v>0</v>
@@ -2992,13 +3009,13 @@
         <v>4</v>
       </c>
       <c r="BK7" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL7" s="2">
         <v>1</v>
       </c>
       <c r="BM7" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:65">
@@ -3009,7 +3026,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -3045,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>132</v>
@@ -3060,13 +3077,13 @@
         <v>1</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="U8" s="2">
-        <v>108338</v>
+        <v>14304</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="W8" s="2">
         <v>1</v>
@@ -3078,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AB8" s="2">
         <v>1</v>
@@ -3126,7 +3143,7 @@
         <v>-361.83</v>
       </c>
       <c r="AU8" s="7" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="AV8" s="2">
         <v>1</v>
@@ -3141,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="AZ8" s="7" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="BA8" s="2">
         <v>0</v>
@@ -3153,7 +3170,7 @@
         <v>-50</v>
       </c>
       <c r="BD8" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="BE8" s="2">
         <v>0</v>
@@ -3174,13 +3191,13 @@
         <v>4</v>
       </c>
       <c r="BK8" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL8" s="2">
         <v>1</v>
       </c>
       <c r="BM8" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:65">
@@ -3191,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -3227,10 +3244,10 @@
         <v>0</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="Q9" s="2">
         <v>1</v>
@@ -3242,13 +3259,13 @@
         <v>1</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="U9" s="2">
         <v>59838</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="W9" s="2">
         <v>1</v>
@@ -3260,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AB9" s="2">
         <v>20</v>
@@ -3308,7 +3325,7 @@
         <v>-361.83</v>
       </c>
       <c r="AU9" s="7" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="AV9" s="2">
         <v>1</v>
@@ -3323,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="AZ9" s="7" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="BA9" s="2">
         <v>0</v>
@@ -3335,7 +3352,7 @@
         <v>-75.54</v>
       </c>
       <c r="BD9" s="7" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="BE9" s="2">
         <v>-1.24</v>
@@ -3356,13 +3373,13 @@
         <v>1.17</v>
       </c>
       <c r="BK9" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL9" s="2">
         <v>1.4</v>
       </c>
       <c r="BM9" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:65">
@@ -3373,7 +3390,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -3409,10 +3426,10 @@
         <v>0</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="Q10" s="2">
         <v>1</v>
@@ -3424,13 +3441,13 @@
         <v>1.17</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="U10" s="2">
         <v>195714</v>
       </c>
       <c r="V10" s="7" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="W10" s="2">
         <v>1</v>
@@ -3442,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AB10" s="2">
         <v>40</v>
@@ -3490,7 +3507,7 @@
         <v>-361.83</v>
       </c>
       <c r="AU10" s="7" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="AV10" s="2">
         <v>1</v>
@@ -3505,7 +3522,7 @@
         <v>0</v>
       </c>
       <c r="AZ10" s="7" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="BA10" s="2">
         <v>0</v>
@@ -3538,13 +3555,13 @@
         <v>4</v>
       </c>
       <c r="BK10" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL10" s="2">
         <v>1</v>
       </c>
       <c r="BM10" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="33" spans="1:65">
@@ -3555,7 +3572,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3573,7 +3590,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="J11" s="2">
         <v>2</v>
@@ -3591,10 +3608,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="Q11" s="2">
         <v>1</v>
@@ -3606,13 +3623,13 @@
         <v>2</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="U11" s="2">
-        <v>114028</v>
+        <v>14304</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="W11" s="2">
         <v>0.72</v>
@@ -3627,7 +3644,7 @@
         <v>1</v>
       </c>
       <c r="AA11" s="7" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="AB11" s="2">
         <v>40</v>
@@ -3675,7 +3692,7 @@
         <v>-361.83</v>
       </c>
       <c r="AU11" s="7" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="AV11" s="2">
         <v>1</v>
@@ -3690,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="AZ11" s="7" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="BA11" s="2">
         <v>0</v>
@@ -3702,7 +3719,7 @@
         <v>-1.73</v>
       </c>
       <c r="BD11" s="7" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="BE11" s="2">
         <v>-0.65</v>
@@ -3723,13 +3740,13 @@
         <v>44.96</v>
       </c>
       <c r="BK11" s="7" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="BL11" s="2">
         <v>1</v>
       </c>
       <c r="BM11" s="7" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1"/>

</xml_diff>

<commit_message>
feat:udpate level change and scene excel change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/SceneEnvironment_场景环境表.xlsx
+++ b/dragon-verse/Excels/SceneEnvironment_场景环境表.xlsx
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="181">
   <si>
     <t>int</t>
   </si>
@@ -639,9 +639,6 @@
   </si>
   <si>
     <t>(R=0.089798,G=0.068563,B=0.117647,A=1.000000)</t>
-  </si>
-  <si>
-    <t>(R=1.000000,G=0.623963,B=0.993237,A=1.000000)</t>
   </si>
   <si>
     <t>(R=0.124772,G=0.088656,B=0.135633,A=1.000000)</t>
@@ -1845,8 +1842,8 @@
   <sheetPr/>
   <dimension ref="A1:BO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16.5"/>
@@ -2895,7 +2892,7 @@
         <v>152</v>
       </c>
       <c r="U7" s="2">
-        <v>14304</v>
+        <v>108338</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>153</v>
@@ -3080,7 +3077,7 @@
         <v>158</v>
       </c>
       <c r="U8" s="2">
-        <v>14304</v>
+        <v>108338</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>159</v>
@@ -3611,7 +3608,7 @@
         <v>173</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="Q11" s="2">
         <v>1</v>
@@ -3623,10 +3620,10 @@
         <v>2</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U11" s="2">
-        <v>14304</v>
+        <v>59821</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>138</v>
@@ -3644,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="AA11" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AB11" s="2">
         <v>40</v>
@@ -3692,7 +3689,7 @@
         <v>-361.83</v>
       </c>
       <c r="AU11" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AV11" s="2">
         <v>1</v>
@@ -3707,19 +3704,19 @@
         <v>0</v>
       </c>
       <c r="AZ11" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="BA11" s="2">
         <v>0</v>
       </c>
       <c r="BB11" s="2">
-        <v>2.52</v>
+        <v>70</v>
       </c>
       <c r="BC11" s="2">
         <v>-1.73</v>
       </c>
       <c r="BD11" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BE11" s="2">
         <v>-0.65</v>
@@ -3737,16 +3734,16 @@
         <v>4368.6</v>
       </c>
       <c r="BJ11" s="2">
-        <v>44.96</v>
+        <v>4</v>
       </c>
       <c r="BK11" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="BL11" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM11" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="BL11" s="2">
-        <v>1</v>
-      </c>
-      <c r="BM11" s="7" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1"/>

</xml_diff>